<commit_message>
Add initial DATASETS rows for ES trades and SpxCombined_pos
</commit_message>
<xml_diff>
--- a/config/run_config.xlsx
+++ b/config/run_config.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-70320" yWindow="3810" windowWidth="45465" windowHeight="24000" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNBOOK" sheetId="1" state="visible" r:id="rId1"/>
@@ -46,7 +45,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'ROBUSTNESS'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'REPORTING'!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -62,7 +61,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,7 +91,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -457,10 +458,16 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.85546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="7.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -500,7 +507,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -613,7 +620,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -799,7 +806,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -842,7 +849,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -905,7 +912,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -958,7 +965,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1001,7 +1008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1049,7 +1056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1137,7 +1144,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1276,14 +1283,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="14.140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="20" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="16.28515625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="19.140625" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="29.5703125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="23.42578125" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="25.7109375" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="8.28515625" bestFit="1" customWidth="1" min="13" max="13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1349,6 +1371,132 @@
       <c r="M1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DB_ES_TRADES</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>intraday_trades</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>databento</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>GLBX.MDP3|ES|trades</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>append</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ts_event</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>intraday_realtime</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>es_trades</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>date,session</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Raw: DBN+zstd split=day under E:\BacktestData\raw\databento\es_trades\&lt;job_id&gt;\; Canonical: Parquet under E:\BacktestData\canonical\es_trades\ partitioned by date+session.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SpxCombined_pos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>daily_series</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>E:\BacktestData\raw\daily\SpxCombined_pos.xlsx</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>append</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>America/New_York</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>eod_20_00_ny</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>spxcombined_pos</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Daily combined positioning (CTA/retail/mutual fund/long-short). Assume populated 20:00 NY time; adjust via DATASETS.known_time_rule if needed.</t>
         </is>
       </c>
     </row>
@@ -1368,7 +1516,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1471,7 +1619,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1569,7 +1717,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1647,7 +1795,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1715,7 +1863,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1783,7 +1931,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Populate INSTRUMENTS for consolidated daily z-score series
</commit_message>
<xml_diff>
--- a/config/run_config.xlsx
+++ b/config/run_config.xlsx
@@ -1283,7 +1283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1410,7 +1410,6 @@
           <t>UTC</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>intraday_realtime</t>
@@ -1497,6 +1496,71 @@
       <c r="M3" t="inlineStr">
         <is>
           <t>Daily combined positioning (CTA/retail/mutual fund/long-short). Assume populated 20:00 NY time; adjust via DATASETS.known_time_rule if needed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>daily_series_wide</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>xlsm</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>E:\BacktestData\raw\consolidated.xlsm</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>append</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>America/New_York</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>eod_20_00_ny</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>daily_series</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Ingest columns: SpxCombined_pos,SpxSystematic_pos,SpxLS_pos,SpxMF_pos,SpxRetail_pos,Spx_NetOptionsPositioning,Spx_DlrGamma,EUshorts_pos,EUetf_pos,EUrp_pos,EUcta_pos,EULS_pos,EUMF_pos,EUComb_pos. Source file: consolidated.xlsm (append-only). Missing values allowed; coverage differs by series.</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1600,6 +1664,706 @@
       <c r="P1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SpxCombined_pos</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SpxCombined_pos</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>SpxCombined_pos</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SpxSystematic_pos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SpxSystematic_pos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>SpxSystematic_pos</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SpxLS_pos</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SpxLS_pos</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>SpxLS_pos</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SpxMF_pos</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SpxMF_pos</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>SpxMF_pos</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SpxRetail_pos</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SpxRetail_pos</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>SpxRetail_pos</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Spx_NetOptionsPositioning</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Spx_NetOptionsPositioning</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Spx_NetOptionsPositioning</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Spx_DlrGamma</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Spx_DlrGamma</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Spx_DlrGamma</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EUshorts_pos</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EUshorts_pos</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>EUshorts_pos</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>EUREX</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>EUetf_pos</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>EUetf_pos</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>EUetf_pos</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>EUREX</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>EUrp_pos</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EUrp_pos</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>EUrp_pos</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>EUREX</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>EUcta_pos</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>EUcta_pos</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>EUcta_pos</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>EUREX</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>EULS_pos</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>EULS_pos</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>EULS_pos</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>EUREX</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>EUMF_pos</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>EUMF_pos</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>EUMF_pos</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>EUREX</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>EUComb_pos</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>EUComb_pos</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>indicator</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>DAILY_CONSOLIDATED_XLSM</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>EUComb_pos</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>EUREX</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Doc cleanup + full spec captured + decisions/progress established
</commit_message>
<xml_diff>
--- a/config/run_config.xlsx
+++ b/config/run_config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-70320" yWindow="3810" windowWidth="45465" windowHeight="24000" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-74130" yWindow="5070" windowWidth="45465" windowHeight="24000" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNBOOK" sheetId="1" state="visible" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'ROBUSTNESS'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'REPORTING'!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1" calcOnSave="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -1430,7 +1430,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Raw: DBN+zstd split=day under E:\BacktestData\raw\databento\es_trades\&lt;job_id&gt;\; Canonical: Parquet under E:\BacktestData\canonical\es_trades\ partitioned by date+session.</t>
+          <t>Raw: DBN+zstd split=day under E:\BacktestData\raw\databento\es_trades\&lt;job_id&gt;\; Canonical: Parquet under E:\BacktestData\canonical\es_trades\ partitioned by date+session. Raw files located at E:\BacktestData\raw\Emini_trade_data\*.trades.dbn; canonical output at E:\BacktestData\canonical\es_trades partitioned by session/date; RTH defined as 09:30-16:00 America/New_York.</t>
         </is>
       </c>
     </row>
@@ -1580,10 +1580,26 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26" bestFit="1" customWidth="1" min="1" max="2"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="27" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="10.140625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="26" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="15.7109375" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="12.140625" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="12" max="13"/>
+    <col width="25.140625" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="32.42578125" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="146.140625" bestFit="1" customWidth="1" min="16" max="16"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1688,17 +1704,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>SpxCombined_pos</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>USD</t>
@@ -1709,8 +1719,6 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -1738,17 +1746,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>SpxSystematic_pos</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>USD</t>
@@ -1759,8 +1761,6 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -1788,17 +1788,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>SpxLS_pos</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>USD</t>
@@ -1809,8 +1803,6 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -1838,17 +1830,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>SpxMF_pos</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>USD</t>
@@ -1859,8 +1845,6 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -1888,17 +1872,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>SpxRetail_pos</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>USD</t>
@@ -1909,8 +1887,6 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -1938,17 +1914,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>Spx_NetOptionsPositioning</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>USD</t>
@@ -1959,8 +1929,6 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -1988,17 +1956,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
           <t>Spx_DlrGamma</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>USD</t>
@@ -2009,8 +1971,6 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -2038,17 +1998,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>EUshorts_pos</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -2059,8 +2013,6 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -2088,17 +2040,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>EUetf_pos</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -2109,8 +2055,6 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -2138,17 +2082,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>EUrp_pos</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -2159,8 +2097,6 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -2188,17 +2124,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
           <t>EUcta_pos</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -2209,8 +2139,6 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -2238,17 +2166,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>EULS_pos</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -2259,8 +2181,6 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -2288,17 +2208,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>EUMF_pos</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -2309,8 +2223,6 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
@@ -2338,17 +2250,11 @@
           <t>DAILY_CONSOLIDATED_XLSM</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>EUComb_pos</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -2359,8 +2265,6 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>

</xml_diff>

<commit_message>
Macro instruments daily ingest + SSD layout in context pack
</commit_message>
<xml_diff>
--- a/config/run_config.xlsx
+++ b/config/run_config.xlsx
@@ -1283,7 +1283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1561,6 +1561,68 @@
       <c r="M4" t="inlineStr">
         <is>
           <t>Ingest columns: SpxCombined_pos,SpxSystematic_pos,SpxLS_pos,SpxMF_pos,SpxRetail_pos,Spx_NetOptionsPositioning,Spx_DlrGamma,EUshorts_pos,EUetf_pos,EUrp_pos,EUcta_pos,EULS_pos,EUMF_pos,EUComb_pos. Source file: consolidated.xlsm (append-only). Missing values allowed; coverage differs by series.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DAILY_MACRO_INSTRUMENTS_XLSX</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>daily_series_wide</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>E:\BacktestData\raw\Macro_Instruments.xlsx</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>full_refresh</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>America/New_York</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1D</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>close</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>daily_series</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Macro instruments workbook. Multi-sheet ingest. First column is date. Drop metadata rows where date cell equals 'DATES' or date cannot be parsed. If sheet has 5 columns total (date + 4 data): base=open, .1=high, .2=low, .3=close. If sheet has 6 columns total (date + 5 data): base=open, .1=high, .2=low, .3=close, .4=volume. If sheet has 2 columns total (date + 1 data): treat as last. Drop rows where all mapped data columns are NA (removes weekends/holidays). Do not forward fill. series_id = '&lt;sheet&gt;|&lt;field&gt;'.
+series_id_prefix_mode: first_data_col
+required_series_ids: SPX Index|close, VIX Index|close, SX5E Index|close, USGG10YR Index|close</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Session 1: build derived bars_1m for ES (FULL + RTH)
- Add tools/add_es_bars_1m_config.py: one-time script that inserts
  ES_BARS_1M into DATASETS sheet and updates INSTRUMENTS ES row
- Add tools/build_derived_bars_1m.py: incremental builder that
  aggregates 1s canonical OHLCV to 1m bars via DuckDB; instrument-
  agnostic (driven by dataset_type='derived_bars' DATASETS rows);
  updates manifest_derived_tables with coverage after each session
- Update config/run_config.xlsx: ES_BARS_1M row added to DATASETS,
  ES row updated in INSTRUMENTS (prices_dataset_id -> ES_BARS_1M)
- Update design/PROGRESS.md: reflect completion of bars_1m build

Build output: 3,113 FULL dates + 2,578 RTH dates written to
E:\BacktestData\derived\bars_1m\ES\{FULL|RTH}\{date}\part-0.parquet
Coverage: 2016-02-23 to 2026-02-23 (FULL), 2016-02-23 to 2026-02-21 (RTH)

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/config/run_config.xlsx
+++ b/config/run_config.xlsx
@@ -1283,7 +1283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1688,6 +1688,72 @@
 rth_start: 09:30
 rth_end: 16:00
 rth_tz: America/New_York</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ES_BARS_1M</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>derived_bars</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>derived</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DB_ES_OHLCV_1S</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>incremental</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>bar_time</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1m</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>event_time</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>bars_1m</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>instrument_id,session,date</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>instrument_id: ES</t>
         </is>
       </c>
     </row>
@@ -2956,7 +3022,27 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>DB_ES_TRADES</t>
+          <t>ES_BARS_1M</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>close</t>
         </is>
       </c>
       <c r="J26" t="n">
@@ -2978,6 +3064,11 @@
       <c r="P26" t="inlineStr">
         <is>
           <t>Placeholder. Trades ingested via DB_ES_TRADES into canonical parquet. Underlying symbols include multiple expiries and spreads. Roll will be configured later (front quarterly roll; exclude spreads unless explicitly enabled).</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>volume</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add big trade events: on-the-fly compute with 3 threshold methods
- src/backtest/data/big_trades.py: get_big_trades() computes real + proxy
  events on-the-fly from canonical parquet; supports fixed_count,
  rolling_pct, z_score thresholds + 5 source modes (real_then_proxy etc.)
- tools/admin/migrate_run_config_add_big_trades_cols.py: adds 3 new
  INSTRUMENTS columns (big_trades_dataset_id, big_trades_proxy_dataset_id,
  big_trades_source_mode)
- tools/admin/add_big_trades_config.py: adds ES_BIG_TRADES + ES_BIG_TRADES_PROXY
  DATASETS rows with threshold config in notes; CLI --instrument-id / --min-size
- Threshold config in DATASETS.notes (method + params); change threshold by
  editing Excel + re-exporting snapshot — no rebuild needed

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/config/run_config.xlsx
+++ b/config/run_config.xlsx
@@ -1283,7 +1283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1891,6 +1891,137 @@
         </is>
       </c>
     </row>
+    <row r="13"/>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ES_BIG_TRADES</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>big_trades</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>canonical</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>DB_ES_TRADES</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>on_the_fly</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ts_event</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>event_time</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>big_trade_events</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>instrument_id,session,date</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>instrument_id: ES
+threshold_method: fixed_count
+min_size: 50</t>
+        </is>
+      </c>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ES_BIG_TRADES_PROXY</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>big_trades_proxy</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>canonical</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>DB_ES_OHLCV_1S</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>on_the_fly</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ts_event</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>1s</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>event_time</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>big_trade_events_proxy</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>instrument_id,session,date</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>instrument_id: ES
+threshold_method: fixed_count
+min_size: 100</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1903,7 +2034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2004,17 +2135,32 @@
           <t>default_execution_price_model</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>big_trades_dataset_id</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>big_trades_proxy_dataset_id</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>big_trades_source_mode</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>volume_col</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>units</t>
         </is>
@@ -2056,7 +2202,7 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2098,7 +2244,7 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2140,7 +2286,7 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2182,7 +2328,7 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2224,7 +2370,7 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2266,7 +2412,7 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2308,7 +2454,7 @@
           <t>NYSE</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2350,7 +2496,7 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2392,7 +2538,7 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2434,7 +2580,7 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2476,7 +2622,7 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2518,7 +2664,7 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2560,7 +2706,7 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2602,7 +2748,7 @@
           <t>EUREX</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="S15" t="inlineStr">
         <is>
           <t>Daily indicator from consolidated.xlsm; units=zscore; timing rule set in DATASETS.known_time_rule; per-series feature lags/transforms go in FEATURE_LIBRARY.</t>
         </is>
@@ -2649,17 +2795,17 @@
           <t>ITRXEXE Corp|close</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>ITRXEXE Corp|volume</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>spread_bp</t>
         </is>
@@ -2706,17 +2852,17 @@
           <t>IBOXHYSE Corp|close</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="S17" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="T17" t="inlineStr">
         <is>
           <t>IBOXHYSE Corp|volume</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
+      <c r="U17" t="inlineStr">
         <is>
           <t>spread_bp</t>
         </is>
@@ -2763,17 +2909,17 @@
           <t>VIX Index|close</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="S18" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="T18" t="inlineStr">
         <is>
           <t>VIX Index|volume</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr">
+      <c r="U18" t="inlineStr">
         <is>
           <t>vol_index</t>
         </is>
@@ -2820,17 +2966,17 @@
           <t>V2X Index|close</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="S19" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="T19" t="inlineStr">
         <is>
           <t>V2X Index|volume</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="U19" t="inlineStr">
         <is>
           <t>vol_index</t>
         </is>
@@ -2877,17 +3023,17 @@
           <t>SPX Index|close</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
+      <c r="S20" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="T20" t="inlineStr">
         <is>
           <t>SPX Index|volume</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr">
+      <c r="U20" t="inlineStr">
         <is>
           <t>index_points</t>
         </is>
@@ -2934,17 +3080,17 @@
           <t>SX5E Index|close</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="S21" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="T21" t="inlineStr">
         <is>
           <t>SX5E Index|volume</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr">
+      <c r="U21" t="inlineStr">
         <is>
           <t>index_points</t>
         </is>
@@ -2991,17 +3137,17 @@
           <t>USGG2YR Index|close</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
+      <c r="S22" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="T22" t="inlineStr">
         <is>
           <t>USGG2YR Index|volume</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
+      <c r="U22" t="inlineStr">
         <is>
           <t>yield_pct</t>
         </is>
@@ -3048,17 +3194,17 @@
           <t>USGG10YR Index|close</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
+      <c r="S23" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
+      <c r="T23" t="inlineStr">
         <is>
           <t>USGG10YR Index|volume</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
+      <c r="U23" t="inlineStr">
         <is>
           <t>yield_pct</t>
         </is>
@@ -3090,12 +3236,12 @@
           <t>SPXAD Index|last</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr">
+      <c r="S24" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="R24" t="inlineStr">
+      <c r="U24" t="inlineStr">
         <is>
           <t>net_advancers</t>
         </is>
@@ -3127,12 +3273,12 @@
           <t>PCUSEQTR Index|last</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
+      <c r="S25" t="inlineStr">
         <is>
           <t>Macro daily series from Macro_Instruments.xlsx; series_id strings stored in *_col fields.</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr">
+      <c r="U25" t="inlineStr">
         <is>
           <t>ratio</t>
         </is>
@@ -3197,10 +3343,25 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
+          <t>ES_BIG_TRADES</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>ES_BIG_TRADES_PROXY</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>real_then_proxy</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
           <t>Placeholder. Trades ingested via DB_ES_TRADES into canonical parquet. Underlying symbols include multiple expiries and spreads. Roll will be configured later (front quarterly roll; exclude spreads unless explicitly enabled).</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr">
+      <c r="T26" t="inlineStr">
         <is>
           <t>volume</t>
         </is>

</xml_diff>

<commit_message>
Add dedicated DATASETS threshold columns for big trade events
Replace free-text notes approach with 5 explicit columns in DATASETS:
threshold_method, threshold_min_size, threshold_pct, threshold_z,
threshold_window_days — each directly editable in Excel.

- schema.py: add 5 threshold columns to DATASETS header list
- migrate_run_config_add_threshold_cols.py: one-time migration; adds
  columns, sets ES_BIG_TRADES (min_size=50) + ES_BIG_TRADES_PROXY
  (min_size=100) defaults, cleans stale threshold lines from notes
- big_trades.py: reads from dedicated columns via _get_threshold_config();
  falls back to notes parsing for backward compat
- add_big_trades_config.py: writes to dedicated columns; notes now
  contains only instrument_id reference

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/config/run_config.xlsx
+++ b/config/run_config.xlsx
@@ -1283,7 +1283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1368,7 +1368,32 @@
           <t>canonical_partition_keys</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>threshold_method</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>threshold_min_size</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>threshold_pct</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>threshold_z</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>threshold_window_days</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -1428,7 +1453,7 @@
           <t>date,session</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>Raw: DBN+zstd split=day under E:\BacktestData\raw\databento\es_trades\&lt;job_id&gt;\; Canonical: Parquet under E:\BacktestData\canonical\es_trades\ partitioned by date+session. Raw files located at E:\BacktestData\raw\Emini_trade_data\*.trades.dbn; canonical output at E:\BacktestData\canonical\es_trades partitioned by session/date; RTH defined as 09:30-16:00 America/New_York.</t>
         </is>
@@ -1493,7 +1518,7 @@
           <t>year</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>Daily combined positioning (CTA/retail/mutual fund/long-short). Assume populated 20:00 NY time; adjust via DATASETS.known_time_rule if needed.</t>
         </is>
@@ -1558,7 +1583,7 @@
           <t>year</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>Ingest columns: SpxCombined_pos,SpxSystematic_pos,SpxLS_pos,SpxMF_pos,SpxRetail_pos,Spx_NetOptionsPositioning,Spx_DlrGamma,EUshorts_pos,EUetf_pos,EUrp_pos,EUcta_pos,EULS_pos,EUMF_pos,EUComb_pos. Source file: consolidated.xlsm (append-only). Missing values allowed; coverage differs by series.</t>
         </is>
@@ -1618,7 +1643,7 @@
           <t>year</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>Macro instruments workbook. Multi-sheet ingest. First column is date. Drop metadata rows where date cell equals 'DATES' or date cannot be parsed. If sheet has 5 columns total (date + 4 data): base=open, .1=high, .2=low, .3=close. If sheet has 6 columns total (date + 5 data): base=open, .1=high, .2=low, .3=close, .4=volume. If sheet has 2 columns total (date + 1 data): treat as last. Drop rows where all mapped data columns are NA (removes weekends/holidays). Do not forward fill. series_id = '&lt;sheet&gt;|&lt;field&gt;'.
 series_id_prefix_mode: first_data_col
@@ -1680,7 +1705,7 @@
           <t>session,date</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>symbol_include_regex: ^ES[HMUZ][0-9]$
 symbol_exclude_contains: -
@@ -1751,7 +1776,7 @@
           <t>instrument_id,session,date</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>instrument_id: ES</t>
         </is>
@@ -1817,7 +1842,7 @@
           <t>instrument_id,session,date</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>instrument_id: ES
 metric_type: footprint</t>
@@ -1884,7 +1909,7 @@
           <t>instrument_id,session,date</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>instrument_id: ES
 metric_type: cvd</t>
@@ -1948,9 +1973,15 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>instrument_id: ES
-threshold_method: fixed_count
-min_size: 50</t>
+          <t>fixed_count</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>50</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>instrument_id: ES</t>
         </is>
       </c>
     </row>
@@ -2016,12 +2047,19 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>instrument_id: ES
-threshold_method: fixed_count
-min_size: 100</t>
-        </is>
-      </c>
-    </row>
+          <t>fixed_count</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>100</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>instrument_id: ES</t>
+        </is>
+      </c>
+    </row>
+    <row r="17"/>
   </sheetData>
   <autoFilter ref="A1:M1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>